<commit_message>
cancer type facet INS - 17 test scripts
</commit_message>
<xml_diff>
--- a/InputFiles/INS/TC04_INS_CancerType-BroadCancerTypes.xlsx
+++ b/InputFiles/INS/TC04_INS_CancerType-BroadCancerTypes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radhakrishnang2/Desktop/Automation/Sep2024/Commons_Automation/InputFiles/INS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC725A3-573E-414D-B196-4AB5821C6833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B474178-D718-BC4A-A7A8-7BD7E9BD3FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="1080" windowWidth="25560" windowHeight="16260" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="4680" yWindow="2640" windowWidth="25560" windowHeight="16260" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,21 +71,6 @@
     <t>TC04_INS_CancerType-BroadCancerTypes_WebData.xlsx</t>
   </si>
   <si>
-    <t>SELECT DISTINCT 
-    prg.program_name AS "Program",
-    prg.website AS "Website",
-    prg.focus_area AS "Focus Area",
-    prg.cancer_type AS "Cancer Type",
-    prg.data_link AS "Data Location Details"
-FROM 
-    df_program prg
-WHERE 
-     prg.cancer_type IN ('Broad Cancer Types')
-ORDER BY 
-    prg.program_name ASC
-LIMIT 100;</t>
-  </si>
-  <si>
     <t>SELECT DISTINCT
     COUNT(DISTINCT prg.program_id) AS "Programs",
     COUNT(DISTINCT prj.project_id) AS "Projects",
@@ -174,14 +159,39 @@
     pub.pmid ASC
 LIMIT 100;</t>
   </si>
+  <si>
+    <t>SELECT DISTINCT 
+    prg.program_name AS "Program",
+    prg.website AS "Website",
+    prg.focus_area AS "Focus Area",
+    prg.cancer_type AS "Cancer Type",
+CASE 
+        WHEN prg.data_link IS NOT NULL THEN prg.website       
+        ELSE prg.data_link
+    END AS "Data Location Details"
+FROM 
+    df_program prg
+WHERE 
+     prg.cancer_type IN ('Broad Cancer Types')
+ORDER BY 
+    LOWER (prg.program_name) ASC
+LIMIT 100;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -234,11 +244,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -564,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -598,11 +611,11 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -616,7 +629,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="356" x14ac:dyDescent="0.2">
@@ -624,7 +637,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -633,7 +646,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -645,7 +658,7 @@
       <c r="C7" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>